<commit_message>
added api structure, added er diagram for database, added folders for bots in future
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28508"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\petProjects\TamagochiMultiplayerGame\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\petProjects\TamagochiService\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C655BD2-CD99-4D7A-B9AA-62FAE1C185EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F4F8FD-98C4-4E25-8D01-0DD0B2AEB2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29865" yWindow="2550" windowWidth="25845" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29865" yWindow="2550" windowWidth="25845" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="план" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
   <si>
     <t>№</t>
   </si>
@@ -205,6 +205,24 @@
   </si>
   <si>
     <t>Это уже под конец, ну либо когда хоть что-то уже будет рабочее готово</t>
+  </si>
+  <si>
+    <t>Реализовано</t>
+  </si>
+  <si>
+    <t>Нет</t>
+  </si>
+  <si>
+    <t>Можно сделать подписочную модель, за которую будут доступны большинство функций, например ты можешь использовать всю одежду, но одежду суперкачества(раритетность вещей) запретить и её придётся только покупать</t>
+  </si>
+  <si>
+    <t>Бот телеграм</t>
+  </si>
+  <si>
+    <t>Бот дискорд</t>
+  </si>
+  <si>
+    <t>Бот вк</t>
   </si>
 </sst>
 </file>
@@ -270,14 +288,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -565,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +620,6 @@
       <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -751,18 +767,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A25F69-F10A-4407-9FC2-86431EE9B575}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="90.140625" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -776,10 +795,13 @@
         <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -793,27 +815,33 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -827,52 +855,64 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -885,8 +925,11 @@
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -900,10 +943,13 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -916,8 +962,11 @@
       <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -931,10 +980,13 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -947,8 +999,11 @@
       <c r="D12" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -961,8 +1016,11 @@
       <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -975,8 +1033,11 @@
       <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -989,8 +1050,11 @@
       <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1004,10 +1068,13 @@
         <v>19</v>
       </c>
       <c r="E16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1019,6 +1086,50 @@
       </c>
       <c r="D17" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added models, added database code for creating
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\petProjects\TamagochiService\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F4F8FD-98C4-4E25-8D01-0DD0B2AEB2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5477A14C-EE78-474B-8FFB-43364B026294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29865" yWindow="2550" windowWidth="25845" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29865" yWindow="2550" windowWidth="25845" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="план" sheetId="1" r:id="rId1"/>
     <sheet name="фичи для реализации" sheetId="2" r:id="rId2"/>
-    <sheet name="стек" sheetId="4" r:id="rId3"/>
-    <sheet name="вопросы" sheetId="3" r:id="rId4"/>
+    <sheet name="Что сделано" sheetId="5" r:id="rId3"/>
+    <sheet name="стек" sheetId="4" r:id="rId4"/>
+    <sheet name="вопросы" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="73">
   <si>
     <t>№</t>
   </si>
@@ -223,6 +224,30 @@
   </si>
   <si>
     <t>Бот вк</t>
+  </si>
+  <si>
+    <t>Для описания слов питомца можно придумать несколько сетов "милый", "грубый", "обычный"</t>
+  </si>
+  <si>
+    <t>Про оплаты всё будет переделыватсья, модель и таблица в бд, сейчас оно просто чтобы было</t>
+  </si>
+  <si>
+    <t>Описаны все модели в API</t>
+  </si>
+  <si>
+    <t>Написан код для создания базы данных при запуске main.py в корне api</t>
+  </si>
+  <si>
+    <t>Написан код для добавления настроек</t>
+  </si>
+  <si>
+    <t>Написана диаграмма ER для бд</t>
+  </si>
+  <si>
+    <t>Статус</t>
+  </si>
+  <si>
+    <t>Есть</t>
   </si>
 </sst>
 </file>
@@ -580,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +618,7 @@
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -606,8 +631,11 @@
       <c r="D1" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -620,8 +648,11 @@
       <c r="D2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -634,12 +665,15 @@
       <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -652,9 +686,9 @@
       <c r="D4" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -667,11 +701,11 @@
       <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -685,7 +719,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -699,7 +733,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -713,7 +747,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -724,7 +758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -735,7 +769,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -745,18 +779,18 @@
       <c r="D11" t="s">
         <v>39</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>58</v>
       </c>
     </row>
@@ -767,10 +801,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A25F69-F10A-4407-9FC2-86431EE9B575}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,6 +1143,9 @@
       <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1120,6 +1157,9 @@
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1130,6 +1170,23 @@
       </c>
       <c r="C21" s="3" t="s">
         <v>29</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1138,6 +1195,64 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30E4ABD-8607-4535-B4DF-6749AA025104}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="77.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78F6CC9-45E2-4EE0-A436-29A18F91FAC4}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1179,12 +1294,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29455EFB-5B0D-41FD-83F3-497299BC909D}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,6 +1330,9 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added start documentation, added columns to db
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\petProjects\TamagochiService\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5477A14C-EE78-474B-8FFB-43364B026294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA495F9F-2FB4-4FC0-87FC-881430CFA542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29865" yWindow="2550" windowWidth="25845" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29865" yWindow="2550" windowWidth="25845" windowHeight="11775" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="план" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>MVP для api питомца</t>
   </si>
   <si>
-    <t>В идеале я всё оранжевое сделаю за завтрашний день, но никаких обещаний</t>
-  </si>
-  <si>
     <t>MVP отдельный сервис для генерации картинок из ассетов</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>Discord-bot</t>
   </si>
   <si>
-    <t>Разработать подробную схему кода, интерфейсов и классов, чтобы всё было унифицировано и дружило друг с другом в любой плоскости</t>
-  </si>
-  <si>
     <t>Docker\Docker-compose файлы</t>
   </si>
   <si>
@@ -248,6 +242,12 @@
   </si>
   <si>
     <t>Есть</t>
+  </si>
+  <si>
+    <t>Разработать подробную схему кода Для API, интерфейсов и классов, чтобы всё было унифицировано и дружило друг с другом в любой плоскости</t>
+  </si>
+  <si>
+    <t>Только сейчас почему-то задалась вопросом как будет выглядеть магазин одежды например(магазин ассетов), мб придётся создать страничку в браузере и в ней можно будет листать и выбирать покупку? Мб как-то в интерфейсе телеграма можно было бы это сделать, у него есть апи для приложений магазинов и оплаты, но что тогда в случае с дискордом делать, потому что там нет такого функционала</t>
   </si>
 </sst>
 </file>
@@ -263,7 +263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,12 +294,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -319,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -605,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +612,7 @@
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -632,10 +626,10 @@
         <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -649,10 +643,10 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -666,14 +660,11 @@
         <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -688,29 +679,29 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -719,12 +710,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -733,7 +724,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -747,51 +738,51 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
         <v>39</v>
       </c>
-      <c r="G11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
         <v>56</v>
-      </c>
-      <c r="G12" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -829,7 +820,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
@@ -849,7 +840,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -869,7 +860,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -889,7 +880,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
         <v>32</v>
@@ -909,7 +900,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -926,7 +917,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -943,7 +934,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -960,7 +951,7 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -977,7 +968,7 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -997,7 +988,7 @@
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1014,7 +1005,7 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
         <v>24</v>
@@ -1034,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1051,7 +1042,7 @@
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1068,7 +1059,7 @@
         <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1085,7 +1076,7 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1102,7 +1093,7 @@
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
         <v>31</v>
@@ -1122,7 +1113,7 @@
         <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,7 +1121,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1138,7 +1129,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
@@ -1152,7 +1143,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
@@ -1166,7 +1157,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>29</v>
@@ -1180,7 +1171,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>29</v>
@@ -1220,7 +1211,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1219,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1236,7 +1227,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1244,7 +1235,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1270,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1278,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1286,7 +1277,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1296,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29455EFB-5B0D-41FD-83F3-497299BC909D}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,10 +1303,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1323,7 +1314,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1331,7 +1322,15 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>